<commit_message>
Updated use case scenarios and backlog
I updated use case scenarios and backlog to make it up to date
</commit_message>
<xml_diff>
--- a/documentation/Product Backlog.xlsx
+++ b/documentation/Product Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pipai/Desktop/CS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pipai/Documents/GitHub/UWG-CS3985-Fall2021-Group5/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C85DC852-DB8E-C54F-941C-AFBB84E305F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEEEF615-8EA0-8542-BD3C-A9AAA9D1D134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15920" xr2:uid="{C66FBFCB-ED40-DA4C-BA83-DB16830430D0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="50">
   <si>
     <t>I want to view my self information</t>
   </si>
@@ -115,12 +115,6 @@
   </si>
   <si>
     <t>So that I can give my suggestion and make  a medical plan for patient based on history and record</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I want to add prescription </t>
-  </si>
-  <si>
-    <t>So that patient can add it for medications</t>
   </si>
   <si>
     <t>I want to enter appointment notes</t>
@@ -549,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F3CB06-B311-BD41-AC1B-E55FCD8F6402}">
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A14" sqref="A14:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -595,7 +589,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
-        <f t="shared" ref="A3:A29" si="0">A2 +1</f>
+        <f t="shared" ref="A3:A28" si="0">A2 +1</f>
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -770,9 +764,9 @@
       <c r="E13" s="1"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
-        <f t="shared" si="0"/>
-        <v>14</v>
+      <c r="A14" s="2" t="e">
+        <f>#REF! +1</f>
+        <v>#REF!</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>20</v>
@@ -786,9 +780,9 @@
       <c r="E14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
-        <f t="shared" si="0"/>
-        <v>15</v>
+      <c r="A15" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>20</v>
@@ -802,9 +796,9 @@
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
-        <f t="shared" si="0"/>
-        <v>16</v>
+      <c r="A16" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>20</v>
@@ -818,9 +812,9 @@
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
-        <f t="shared" si="0"/>
-        <v>17</v>
+      <c r="A17" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>20</v>
@@ -834,31 +828,31 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
-        <f t="shared" si="0"/>
-        <v>18</v>
+      <c r="A18" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
       <c r="C19" s="1" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>40</v>
@@ -866,12 +860,12 @@
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
-        <f t="shared" si="0"/>
-        <v>20</v>
+      <c r="A20" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>41</v>
@@ -882,12 +876,12 @@
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
-        <f t="shared" si="0"/>
-        <v>21</v>
+      <c r="A21" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>43</v>
@@ -898,132 +892,116 @@
       <c r="E21" s="1"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
-        <f t="shared" si="0"/>
-        <v>22</v>
+      <c r="A22" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="D23" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
-        <f t="shared" si="0"/>
-        <v>24</v>
+      <c r="A24" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E26" s="1"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
-        <f t="shared" si="0"/>
-        <v>27</v>
+      <c r="A27" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
-        <f t="shared" si="0"/>
-        <v>28</v>
+      <c r="A28" s="2" t="e">
+        <f t="shared" si="0"/>
+        <v>#REF!</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E29" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>